<commit_message>
dataGateway added for vis
</commit_message>
<xml_diff>
--- a/configuration/configuration.xlsx
+++ b/configuration/configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias\workspace\venice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias\workspace\venice\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -386,7 +386,7 @@
   <dimension ref="A1:U57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +485,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:O10" si="0">$A10*$D$1</f>
+        <f t="shared" ref="E10:U10" si="0">$A10*$D$1</f>
         <v>0</v>
       </c>
       <c r="F10">
@@ -528,6 +528,30 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -543,37 +567,71 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>400</v>
+        <v>235</v>
       </c>
       <c r="F11">
-        <v>800</v>
+        <f>E11+235</f>
+        <v>470</v>
       </c>
       <c r="G11">
-        <v>1200</v>
+        <f t="shared" ref="G11:U11" si="1">F11+235</f>
+        <v>705</v>
       </c>
       <c r="H11">
-        <v>1600</v>
+        <f t="shared" si="1"/>
+        <v>940</v>
       </c>
       <c r="I11">
-        <v>2000</v>
+        <f t="shared" si="1"/>
+        <v>1175</v>
       </c>
       <c r="J11">
-        <v>2400</v>
+        <f>I11+235+235</f>
+        <v>1645</v>
       </c>
       <c r="K11">
-        <v>2800</v>
+        <f t="shared" si="1"/>
+        <v>1880</v>
       </c>
       <c r="L11">
-        <v>3200</v>
+        <f t="shared" si="1"/>
+        <v>2115</v>
       </c>
       <c r="M11">
-        <v>3600</v>
+        <f t="shared" si="1"/>
+        <v>2350</v>
       </c>
       <c r="N11">
-        <v>4000</v>
+        <f t="shared" si="1"/>
+        <v>2585</v>
       </c>
       <c r="O11">
-        <v>4400</v>
+        <f t="shared" si="1"/>
+        <v>2820</v>
+      </c>
+      <c r="P11">
+        <f>O11+235+235</f>
+        <v>3290</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>3525</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>3760</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>3995</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>4230</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="1"/>
+        <v>4465</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -622,6 +680,24 @@
       <c r="O12">
         <v>3500</v>
       </c>
+      <c r="P12">
+        <v>3500</v>
+      </c>
+      <c r="Q12">
+        <v>3500</v>
+      </c>
+      <c r="R12">
+        <v>3500</v>
+      </c>
+      <c r="S12">
+        <v>3500</v>
+      </c>
+      <c r="T12">
+        <v>3500</v>
+      </c>
+      <c r="U12">
+        <v>3500</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -638,47 +714,71 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:O13" si="1">$A13</f>
+        <f t="shared" ref="E13:U13" si="2">$A13</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -729,6 +829,24 @@
       <c r="O14">
         <v>10.999999999999998</v>
       </c>
+      <c r="P14">
+        <v>12</v>
+      </c>
+      <c r="Q14">
+        <v>13</v>
+      </c>
+      <c r="R14">
+        <v>14</v>
+      </c>
+      <c r="S14">
+        <v>15</v>
+      </c>
+      <c r="T14">
+        <v>16</v>
+      </c>
+      <c r="U14">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -741,40 +859,58 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="P15">
+        <v>90</v>
+      </c>
+      <c r="Q15">
+        <v>90</v>
+      </c>
+      <c r="R15">
+        <v>90</v>
+      </c>
+      <c r="S15">
+        <v>90</v>
+      </c>
+      <c r="T15">
+        <v>90</v>
+      </c>
+      <c r="U15">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -823,8 +959,26 @@
       <c r="O16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>45</v>
+      </c>
+      <c r="Q16">
+        <v>45</v>
+      </c>
+      <c r="R16">
+        <v>45</v>
+      </c>
+      <c r="S16">
+        <v>45</v>
+      </c>
+      <c r="T16">
+        <v>45</v>
+      </c>
+      <c r="U16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -870,8 +1024,26 @@
       <c r="O17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -909,16 +1081,34 @@
         <v>10</v>
       </c>
       <c r="M18">
-        <v>11</v>
+        <v>10.999999999999998</v>
       </c>
       <c r="N18">
         <v>12</v>
       </c>
       <c r="O18">
-        <v>13.000000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>13.000000000000002</v>
+      </c>
+      <c r="P18">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="Q18">
+        <v>15.000000000000005</v>
+      </c>
+      <c r="R18">
+        <v>16.000000000000007</v>
+      </c>
+      <c r="S18">
+        <v>17.000000000000007</v>
+      </c>
+      <c r="T18">
+        <v>18.000000000000011</v>
+      </c>
+      <c r="U18">
+        <v>19.000000000000014</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -964,8 +1154,26 @@
       <c r="O19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1003,16 +1211,34 @@
         <v>10</v>
       </c>
       <c r="M20">
-        <v>11</v>
+        <v>10.999999999999998</v>
       </c>
       <c r="N20">
         <v>12</v>
       </c>
       <c r="O20">
-        <v>13.000000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>13.000000000000002</v>
+      </c>
+      <c r="P20">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="Q20">
+        <v>15.000000000000005</v>
+      </c>
+      <c r="R20">
+        <v>16.000000000000007</v>
+      </c>
+      <c r="S20">
+        <v>17.000000000000007</v>
+      </c>
+      <c r="T20">
+        <v>18.000000000000011</v>
+      </c>
+      <c r="U20">
+        <v>19.000000000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1058,8 +1284,26 @@
       <c r="O21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1071,51 +1315,75 @@
         <v>1829</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:O22" si="2">$A22*$D$1</f>
+        <f t="shared" ref="E22:U22" si="3">$A22*$D$1</f>
         <v>1829</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="G22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="J22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="K22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="L22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="M22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="N22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
       <c r="O22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1829</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>1829</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="3"/>
+        <v>1829</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="3"/>
+        <v>1829</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="3"/>
+        <v>1829</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="3"/>
+        <v>1829</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="3"/>
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1123,43 +1391,79 @@
         <v>2</v>
       </c>
       <c r="D23">
+        <f>D11</f>
         <v>0</v>
       </c>
       <c r="E23">
-        <v>400</v>
+        <f t="shared" ref="E23:U23" si="4">E11</f>
+        <v>235</v>
       </c>
       <c r="F23">
-        <v>800</v>
+        <f t="shared" si="4"/>
+        <v>470</v>
       </c>
       <c r="G23">
-        <v>1200</v>
+        <f t="shared" si="4"/>
+        <v>705</v>
       </c>
       <c r="H23">
-        <v>1600</v>
+        <f t="shared" si="4"/>
+        <v>940</v>
       </c>
       <c r="I23">
-        <v>2000</v>
+        <f t="shared" si="4"/>
+        <v>1175</v>
       </c>
       <c r="J23">
-        <v>2400</v>
+        <f t="shared" si="4"/>
+        <v>1645</v>
       </c>
       <c r="K23">
-        <v>2800</v>
+        <f t="shared" si="4"/>
+        <v>1880</v>
       </c>
       <c r="L23">
-        <v>3200</v>
+        <f t="shared" si="4"/>
+        <v>2115</v>
       </c>
       <c r="M23">
-        <v>3600</v>
+        <f t="shared" si="4"/>
+        <v>2350</v>
       </c>
       <c r="N23">
-        <v>4000</v>
+        <f t="shared" si="4"/>
+        <v>2585</v>
       </c>
       <c r="O23">
-        <v>4400</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2820</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>3290</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="4"/>
+        <v>3525</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="4"/>
+        <v>3760</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="4"/>
+        <v>3995</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="4"/>
+        <v>4230</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="4"/>
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1202,8 +1506,26 @@
       <c r="O24">
         <v>3500</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>3500</v>
+      </c>
+      <c r="Q24">
+        <v>3500</v>
+      </c>
+      <c r="R24">
+        <v>3500</v>
+      </c>
+      <c r="S24">
+        <v>3500</v>
+      </c>
+      <c r="T24">
+        <v>3500</v>
+      </c>
+      <c r="U24">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1215,51 +1537,75 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25:O25" si="3">$A25</f>
+        <f t="shared" ref="E25:U25" si="5">$A25</f>
         <v>1</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O25">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1267,44 +1613,79 @@
         <v>5</v>
       </c>
       <c r="D26">
-        <f>D$9</f>
+        <f>D14</f>
         <v>0</v>
       </c>
       <c r="E26">
+        <f t="shared" ref="E26:U26" si="6">E14</f>
         <v>1.0000000000000004</v>
       </c>
       <c r="F26">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G26">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="H26">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I26">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="J26">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="K26">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="L26">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="M26">
+        <f t="shared" si="6"/>
         <v>8.9999999999999982</v>
       </c>
       <c r="N26">
+        <f t="shared" si="6"/>
         <v>9.9999999999999982</v>
       </c>
       <c r="O26">
+        <f t="shared" si="6"/>
         <v>10.999999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1312,43 +1693,61 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="P27">
+        <v>90</v>
+      </c>
+      <c r="Q27">
+        <v>90</v>
+      </c>
+      <c r="R27">
+        <v>90</v>
+      </c>
+      <c r="S27">
+        <v>90</v>
+      </c>
+      <c r="T27">
+        <v>90</v>
+      </c>
+      <c r="U27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1391,8 +1790,26 @@
       <c r="O28">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <v>45</v>
+      </c>
+      <c r="Q28">
+        <v>45</v>
+      </c>
+      <c r="R28">
+        <v>45</v>
+      </c>
+      <c r="S28">
+        <v>45</v>
+      </c>
+      <c r="T28">
+        <v>45</v>
+      </c>
+      <c r="U28">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1435,8 +1852,26 @@
       <c r="O29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1444,43 +1879,61 @@
         <v>10</v>
       </c>
       <c r="D30">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E30">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F30">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G30">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H30">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I30">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J30">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="K30">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="L30">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="M30">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="N30">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="O30">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="P30">
+        <v>32</v>
+      </c>
+      <c r="Q30">
+        <v>33</v>
+      </c>
+      <c r="R30">
+        <v>34</v>
+      </c>
+      <c r="S30">
+        <v>35</v>
+      </c>
+      <c r="T30">
+        <v>36</v>
+      </c>
+      <c r="U30">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1523,8 +1976,26 @@
       <c r="O31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1532,43 +2003,61 @@
         <v>12</v>
       </c>
       <c r="D32">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E32">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F32">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G32">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H32">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I32">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J32">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="K32">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="L32">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="M32">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="N32">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="O32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="P32">
+        <v>32</v>
+      </c>
+      <c r="Q32">
+        <v>33</v>
+      </c>
+      <c r="R32">
+        <v>34</v>
+      </c>
+      <c r="S32">
+        <v>35</v>
+      </c>
+      <c r="T32">
+        <v>36</v>
+      </c>
+      <c r="U32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -1614,8 +2103,26 @@
       <c r="O33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1627,27 +2134,75 @@
         <v>3658</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:I34" si="4">$A34*$D$1</f>
+        <f t="shared" ref="E34:U34" si="7">$A34*$D$1</f>
         <v>3658</v>
       </c>
       <c r="F34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3658</v>
       </c>
       <c r="G34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3658</v>
       </c>
       <c r="H34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3658</v>
       </c>
       <c r="I34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3658</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="7"/>
+        <v>3658</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1655,25 +2210,79 @@
         <v>2</v>
       </c>
       <c r="D35">
+        <f>D23</f>
         <v>0</v>
       </c>
       <c r="E35">
-        <v>400</v>
+        <f t="shared" ref="E35:U35" si="8">E23</f>
+        <v>235</v>
       </c>
       <c r="F35">
-        <v>800</v>
+        <f t="shared" si="8"/>
+        <v>470</v>
       </c>
       <c r="G35">
-        <v>1200</v>
+        <f t="shared" si="8"/>
+        <v>705</v>
       </c>
       <c r="H35">
-        <v>1600</v>
+        <f t="shared" si="8"/>
+        <v>940</v>
       </c>
       <c r="I35">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1175</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="8"/>
+        <v>1645</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="8"/>
+        <v>1880</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="8"/>
+        <v>2115</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="8"/>
+        <v>2350</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="8"/>
+        <v>2585</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="8"/>
+        <v>2820</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="8"/>
+        <v>3290</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="8"/>
+        <v>3525</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="8"/>
+        <v>3760</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="8"/>
+        <v>3995</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="8"/>
+        <v>4230</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="8"/>
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1698,8 +2307,44 @@
       <c r="I36">
         <v>3500</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>3500</v>
+      </c>
+      <c r="K36">
+        <v>3500</v>
+      </c>
+      <c r="L36">
+        <v>3500</v>
+      </c>
+      <c r="M36">
+        <v>3500</v>
+      </c>
+      <c r="N36">
+        <v>3500</v>
+      </c>
+      <c r="O36">
+        <v>3500</v>
+      </c>
+      <c r="P36">
+        <v>3500</v>
+      </c>
+      <c r="Q36">
+        <v>3500</v>
+      </c>
+      <c r="R36">
+        <v>3500</v>
+      </c>
+      <c r="S36">
+        <v>3500</v>
+      </c>
+      <c r="T36">
+        <v>3500</v>
+      </c>
+      <c r="U36">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1711,27 +2356,75 @@
         <v>2</v>
       </c>
       <c r="E37">
-        <f t="shared" ref="E37:I37" si="5">$A37</f>
+        <f t="shared" ref="E37:U37" si="9">$A37</f>
         <v>2</v>
       </c>
       <c r="F37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="G37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="H37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="I37">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1739,31 +2432,79 @@
         <v>5</v>
       </c>
       <c r="D38">
-        <f>D$9</f>
+        <f>D26</f>
         <v>0</v>
       </c>
       <c r="E38">
-        <f t="shared" ref="E38:I38" si="6">E$9</f>
-        <v>1</v>
+        <f t="shared" ref="E38:U38" si="10">E26</f>
+        <v>1.0000000000000004</v>
       </c>
       <c r="F38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="G38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="H38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="I38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="10"/>
+        <v>8.9999999999999982</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="10"/>
+        <v>9.9999999999999982</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="10"/>
+        <v>10.999999999999998</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="10"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1771,25 +2512,61 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="J39">
+        <v>90</v>
+      </c>
+      <c r="K39">
+        <v>90</v>
+      </c>
+      <c r="L39">
+        <v>90</v>
+      </c>
+      <c r="M39">
+        <v>90</v>
+      </c>
+      <c r="N39">
+        <v>90</v>
+      </c>
+      <c r="O39">
+        <v>90</v>
+      </c>
+      <c r="P39">
+        <v>90</v>
+      </c>
+      <c r="Q39">
+        <v>90</v>
+      </c>
+      <c r="R39">
+        <v>90</v>
+      </c>
+      <c r="S39">
+        <v>90</v>
+      </c>
+      <c r="T39">
+        <v>90</v>
+      </c>
+      <c r="U39">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1814,8 +2591,44 @@
       <c r="I40">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>45</v>
+      </c>
+      <c r="K40">
+        <v>45</v>
+      </c>
+      <c r="L40">
+        <v>45</v>
+      </c>
+      <c r="M40">
+        <v>45</v>
+      </c>
+      <c r="N40">
+        <v>45</v>
+      </c>
+      <c r="O40">
+        <v>45</v>
+      </c>
+      <c r="P40">
+        <v>45</v>
+      </c>
+      <c r="Q40">
+        <v>45</v>
+      </c>
+      <c r="R40">
+        <v>45</v>
+      </c>
+      <c r="S40">
+        <v>45</v>
+      </c>
+      <c r="T40">
+        <v>45</v>
+      </c>
+      <c r="U40">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1823,25 +2636,61 @@
         <v>9</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>2</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="O41">
+        <v>2</v>
+      </c>
+      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41">
+        <v>2</v>
+      </c>
+      <c r="S41">
+        <v>2</v>
+      </c>
+      <c r="T41">
+        <v>2</v>
+      </c>
+      <c r="U41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1849,25 +2698,61 @@
         <v>10</v>
       </c>
       <c r="D42">
-        <v>26</v>
+        <v>1.9999999999999993</v>
       </c>
       <c r="E42">
-        <v>27</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="F42">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G42">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="H42">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="I42">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="J42">
+        <v>8</v>
+      </c>
+      <c r="K42">
+        <v>9</v>
+      </c>
+      <c r="L42">
+        <v>10</v>
+      </c>
+      <c r="M42">
+        <v>10.999999999999998</v>
+      </c>
+      <c r="N42">
+        <v>12</v>
+      </c>
+      <c r="O42">
+        <v>13.000000000000002</v>
+      </c>
+      <c r="P42">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="Q42">
+        <v>15.000000000000005</v>
+      </c>
+      <c r="R42">
+        <v>16.000000000000007</v>
+      </c>
+      <c r="S42">
+        <v>17.000000000000007</v>
+      </c>
+      <c r="T42">
+        <v>18.000000000000011</v>
+      </c>
+      <c r="U42">
+        <v>19.000000000000014</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1875,25 +2760,61 @@
         <v>11</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>3</v>
+      </c>
+      <c r="K43">
+        <v>3</v>
+      </c>
+      <c r="L43">
+        <v>3</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="N43">
+        <v>3</v>
+      </c>
+      <c r="O43">
+        <v>3</v>
+      </c>
+      <c r="P43">
+        <v>3</v>
+      </c>
+      <c r="Q43">
+        <v>3</v>
+      </c>
+      <c r="R43">
+        <v>3</v>
+      </c>
+      <c r="S43">
+        <v>3</v>
+      </c>
+      <c r="T43">
+        <v>3</v>
+      </c>
+      <c r="U43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1901,25 +2822,61 @@
         <v>12</v>
       </c>
       <c r="D44">
-        <v>26</v>
+        <v>1.9999999999999993</v>
       </c>
       <c r="E44">
-        <v>27</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="F44">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G44">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="H44">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="I44">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="J44">
+        <v>8</v>
+      </c>
+      <c r="K44">
+        <v>9</v>
+      </c>
+      <c r="L44">
+        <v>10</v>
+      </c>
+      <c r="M44">
+        <v>10.999999999999998</v>
+      </c>
+      <c r="N44">
+        <v>12</v>
+      </c>
+      <c r="O44">
+        <v>13.000000000000002</v>
+      </c>
+      <c r="P44">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="Q44">
+        <v>15.000000000000005</v>
+      </c>
+      <c r="R44">
+        <v>16.000000000000007</v>
+      </c>
+      <c r="S44">
+        <v>17.000000000000007</v>
+      </c>
+      <c r="T44">
+        <v>18.000000000000011</v>
+      </c>
+      <c r="U44">
+        <v>19.000000000000014</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1944,101 +2901,857 @@
       <c r="I45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f>$A46*$D$1</f>
+        <v>5487</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ref="E46:U46" si="11">$A46*$D$1</f>
+        <v>5487</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="11"/>
+        <v>5487</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
       <c r="B47" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f>D35</f>
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ref="E47:U47" si="12">E35</f>
+        <v>235</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="12"/>
+        <v>470</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="12"/>
+        <v>705</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="12"/>
+        <v>940</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="12"/>
+        <v>1175</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="12"/>
+        <v>1645</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="12"/>
+        <v>1880</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="12"/>
+        <v>2115</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="12"/>
+        <v>2350</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="12"/>
+        <v>2585</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="12"/>
+        <v>2820</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="12"/>
+        <v>3290</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="12"/>
+        <v>3525</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="12"/>
+        <v>3760</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="12"/>
+        <v>3995</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="12"/>
+        <v>4230</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="12"/>
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>3500</v>
+      </c>
+      <c r="E48">
+        <v>3500</v>
+      </c>
+      <c r="F48">
+        <v>3500</v>
+      </c>
+      <c r="G48">
+        <v>3500</v>
+      </c>
+      <c r="H48">
+        <v>3500</v>
+      </c>
+      <c r="I48">
+        <v>3500</v>
+      </c>
+      <c r="J48">
+        <v>3500</v>
+      </c>
+      <c r="K48">
+        <v>3500</v>
+      </c>
+      <c r="L48">
+        <v>3500</v>
+      </c>
+      <c r="M48">
+        <v>3500</v>
+      </c>
+      <c r="N48">
+        <v>3500</v>
+      </c>
+      <c r="O48">
+        <v>3500</v>
+      </c>
+      <c r="P48">
+        <v>3500</v>
+      </c>
+      <c r="Q48">
+        <v>3500</v>
+      </c>
+      <c r="R48">
+        <v>3500</v>
+      </c>
+      <c r="S48">
+        <v>3500</v>
+      </c>
+      <c r="T48">
+        <v>3500</v>
+      </c>
+      <c r="U48">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f>$A49</f>
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <f t="shared" ref="E49:U49" si="13">$A49</f>
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f>D38</f>
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <f t="shared" ref="E50:U50" si="14">E38</f>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="14"/>
+        <v>8.9999999999999982</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="14"/>
+        <v>9.9999999999999982</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="14"/>
+        <v>10.999999999999998</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="14"/>
+        <v>16</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="14"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>90</v>
+      </c>
+      <c r="E51">
+        <v>90</v>
+      </c>
+      <c r="F51">
+        <v>90</v>
+      </c>
+      <c r="G51">
+        <v>90</v>
+      </c>
+      <c r="H51">
+        <v>90</v>
+      </c>
+      <c r="I51">
+        <v>90</v>
+      </c>
+      <c r="J51">
+        <v>90</v>
+      </c>
+      <c r="K51">
+        <v>90</v>
+      </c>
+      <c r="L51">
+        <v>90</v>
+      </c>
+      <c r="M51">
+        <v>90</v>
+      </c>
+      <c r="N51">
+        <v>90</v>
+      </c>
+      <c r="O51">
+        <v>90</v>
+      </c>
+      <c r="P51">
+        <v>90</v>
+      </c>
+      <c r="Q51">
+        <v>90</v>
+      </c>
+      <c r="R51">
+        <v>90</v>
+      </c>
+      <c r="S51">
+        <v>90</v>
+      </c>
+      <c r="T51">
+        <v>90</v>
+      </c>
+      <c r="U51">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>45</v>
+      </c>
+      <c r="E52">
+        <v>45</v>
+      </c>
+      <c r="F52">
+        <v>45</v>
+      </c>
+      <c r="G52">
+        <v>45</v>
+      </c>
+      <c r="H52">
+        <v>45</v>
+      </c>
+      <c r="I52">
+        <v>45</v>
+      </c>
+      <c r="J52">
+        <v>45</v>
+      </c>
+      <c r="K52">
+        <v>45</v>
+      </c>
+      <c r="L52">
+        <v>45</v>
+      </c>
+      <c r="M52">
+        <v>45</v>
+      </c>
+      <c r="N52">
+        <v>45</v>
+      </c>
+      <c r="O52">
+        <v>45</v>
+      </c>
+      <c r="P52">
+        <v>45</v>
+      </c>
+      <c r="Q52">
+        <v>45</v>
+      </c>
+      <c r="R52">
+        <v>45</v>
+      </c>
+      <c r="S52">
+        <v>45</v>
+      </c>
+      <c r="T52">
+        <v>45</v>
+      </c>
+      <c r="U52">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53">
+        <v>2</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <v>2</v>
+      </c>
+      <c r="N53">
+        <v>2</v>
+      </c>
+      <c r="O53">
+        <v>2</v>
+      </c>
+      <c r="P53">
+        <v>2</v>
+      </c>
+      <c r="Q53">
+        <v>2</v>
+      </c>
+      <c r="R53">
+        <v>2</v>
+      </c>
+      <c r="S53">
+        <v>2</v>
+      </c>
+      <c r="T53">
+        <v>2</v>
+      </c>
+      <c r="U53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>20</v>
+      </c>
+      <c r="E54">
+        <v>21</v>
+      </c>
+      <c r="F54">
+        <v>22</v>
+      </c>
+      <c r="G54">
+        <v>23</v>
+      </c>
+      <c r="H54">
+        <v>24</v>
+      </c>
+      <c r="I54">
+        <v>25</v>
+      </c>
+      <c r="J54">
+        <v>26</v>
+      </c>
+      <c r="K54">
+        <v>27</v>
+      </c>
+      <c r="L54">
+        <v>28</v>
+      </c>
+      <c r="M54">
+        <v>29</v>
+      </c>
+      <c r="N54">
+        <v>30</v>
+      </c>
+      <c r="O54">
+        <v>31</v>
+      </c>
+      <c r="P54">
+        <v>32</v>
+      </c>
+      <c r="Q54">
+        <v>33</v>
+      </c>
+      <c r="R54">
+        <v>34</v>
+      </c>
+      <c r="S54">
+        <v>35</v>
+      </c>
+      <c r="T54">
+        <v>36</v>
+      </c>
+      <c r="U54">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <v>3</v>
+      </c>
+      <c r="M55">
+        <v>3</v>
+      </c>
+      <c r="N55">
+        <v>3</v>
+      </c>
+      <c r="O55">
+        <v>3</v>
+      </c>
+      <c r="P55">
+        <v>3</v>
+      </c>
+      <c r="Q55">
+        <v>3</v>
+      </c>
+      <c r="R55">
+        <v>3</v>
+      </c>
+      <c r="S55">
+        <v>3</v>
+      </c>
+      <c r="T55">
+        <v>3</v>
+      </c>
+      <c r="U55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>20</v>
+      </c>
+      <c r="E56">
+        <v>21</v>
+      </c>
+      <c r="F56">
+        <v>22</v>
+      </c>
+      <c r="G56">
+        <v>23</v>
+      </c>
+      <c r="H56">
+        <v>24</v>
+      </c>
+      <c r="I56">
+        <v>25</v>
+      </c>
+      <c r="J56">
+        <v>26</v>
+      </c>
+      <c r="K56">
+        <v>27</v>
+      </c>
+      <c r="L56">
+        <v>28</v>
+      </c>
+      <c r="M56">
+        <v>29</v>
+      </c>
+      <c r="N56">
+        <v>30</v>
+      </c>
+      <c r="O56">
+        <v>31</v>
+      </c>
+      <c r="P56">
+        <v>32</v>
+      </c>
+      <c r="Q56">
+        <v>33</v>
+      </c>
+      <c r="R56">
+        <v>34</v>
+      </c>
+      <c r="S56">
+        <v>35</v>
+      </c>
+      <c r="T56">
+        <v>36</v>
+      </c>
+      <c r="U56">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="P57">
+        <v>1</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>